<commit_message>
conversion between excel and python data
</commit_message>
<xml_diff>
--- a/english/pythonnet/developer-guide/conversions/convert-excel-to-list/sample_data.xlsx
+++ b/english/pythonnet/developer-guide/conversions/convert-excel-to-list/sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VSCodeCellsDoc\Aspose.Cells-Doc-md\english\pythonnet\developer-guide\conversions\convert-excel-to-list\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\PythonWorkspace\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDCCFCD7-5573-4BDB-A3EC-62C31D09EA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C60055-76D1-4DDF-B33E-B132F07AF135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="16">
   <si>
     <t>City</t>
   </si>
@@ -422,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -548,9 +548,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -603,17 +605,6 @@
         <v>3055</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5">
-        <v>3090</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>